<commit_message>
IMPORTANT UPDATE: Update of the HK map
</commit_message>
<xml_diff>
--- a/Source/MetroSystem/data/stations_HK.xlsx
+++ b/Source/MetroSystem/data/stations_HK.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WANG\Desktop\CS3343_Group6-lw-dev\Source\MetroSystem\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\城大\课程\Year 3 Sem A\CS3343\CS3343_Group6\Source\MetroSystem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F042D8A3-F156-4462-AA2A-3631F35F4E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECB0EB0-8AE5-4299-B354-04899A025C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="2505" windowWidth="20220" windowHeight="8168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11280" yWindow="2484" windowWidth="11052" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1042,17 +1042,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1083,7 +1083,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1363,16 +1363,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.46484375" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>150</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>151</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>152</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1672,13 +1672,13 @@
         <v>38</v>
       </c>
       <c r="D18">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="E18">
         <v>733</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>49</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>70</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>182</v>
       </c>
@@ -1927,13 +1927,13 @@
         <v>179</v>
       </c>
       <c r="D33">
-        <v>880</v>
+        <v>891</v>
       </c>
       <c r="E33">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>183</v>
       </c>
@@ -1944,13 +1944,13 @@
         <v>180</v>
       </c>
       <c r="D34">
-        <v>880</v>
+        <v>940</v>
       </c>
       <c r="E34">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>81</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>88</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>93</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>99</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>102</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>104</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>108</v>
       </c>
@@ -2165,13 +2165,13 @@
         <v>107</v>
       </c>
       <c r="D47">
-        <v>1231</v>
+        <v>1292</v>
       </c>
       <c r="E47">
         <v>432</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -2182,13 +2182,13 @@
         <v>110</v>
       </c>
       <c r="D48">
-        <v>1231</v>
+        <v>1324</v>
       </c>
       <c r="E48">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -2199,13 +2199,13 @@
         <v>114</v>
       </c>
       <c r="D49">
-        <v>1231</v>
+        <v>1324</v>
       </c>
       <c r="E49">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>116</v>
       </c>
@@ -2216,13 +2216,13 @@
         <v>117</v>
       </c>
       <c r="D50">
-        <v>1231</v>
+        <v>1324</v>
       </c>
       <c r="E50">
         <v>481</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>119</v>
       </c>
@@ -2233,13 +2233,13 @@
         <v>118</v>
       </c>
       <c r="D51">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="E51">
         <v>520</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>120</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>125</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>126</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>129</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>132</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>133</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>140</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>141</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>142</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>161</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>162</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>163</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>164</v>
       </c>
@@ -2460,7 +2460,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>216</v>
       </c>
@@ -2474,10 +2474,10 @@
         <v>127</v>
       </c>
       <c r="E65">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>217</v>
       </c>
@@ -2491,10 +2491,10 @@
         <v>127</v>
       </c>
       <c r="E66">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>218</v>
       </c>
@@ -2505,13 +2505,13 @@
         <v>168</v>
       </c>
       <c r="D67">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="E67">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>219</v>
       </c>
@@ -2522,13 +2522,13 @@
         <v>170</v>
       </c>
       <c r="D68">
-        <v>179</v>
+        <v>203</v>
       </c>
       <c r="E68">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>220</v>
       </c>
@@ -2539,13 +2539,13 @@
         <v>172</v>
       </c>
       <c r="D69">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="E69">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>221</v>
       </c>
@@ -2556,13 +2556,13 @@
         <v>173</v>
       </c>
       <c r="D70">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="E70">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>222</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>223</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>224</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>225</v>
       </c>
@@ -2627,10 +2627,10 @@
         <v>849</v>
       </c>
       <c r="E74">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>226</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>227</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>228</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>229</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>230</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>231</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>232</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>233</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>234</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>235</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>236</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>237</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>238</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>259</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>260</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>261</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>262</v>
       </c>
@@ -2916,10 +2916,10 @@
         <v>890</v>
       </c>
       <c r="E91">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>263</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>264</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>265</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>266</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>267</v>
       </c>
@@ -3004,7 +3004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>268</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>269</v>
       </c>

</xml_diff>